<commit_message>
Clean-up all processing scripts.
</commit_message>
<xml_diff>
--- a/data/interim/process_node_eval.xlsx
+++ b/data/interim/process_node_eval.xlsx
@@ -486,12 +486,12 @@
     <row r="1">
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>timeint</t>
+          <t>timeint_label</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>900-4500</t>
+          <t>6:00-7:00 am</t>
         </is>
       </c>
       <c r="H1" s="1" t="n"/>
@@ -500,7 +500,7 @@
       <c r="K1" s="1" t="n"/>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>4500-8100</t>
+          <t>7:00-8:00 am</t>
         </is>
       </c>
       <c r="M1" s="1" t="n"/>
@@ -509,7 +509,7 @@
       <c r="P1" s="1" t="n"/>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>8100-11700</t>
+          <t>8:00-9:00 am</t>
         </is>
       </c>
       <c r="R1" s="1" t="n"/>
@@ -518,7 +518,7 @@
       <c r="U1" s="1" t="n"/>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>11700-12600</t>
+          <t>9:00-9:15 am</t>
         </is>
       </c>
       <c r="W1" s="1" t="n"/>

</xml_diff>